<commit_message>
dashboard figs data repository headings updated
</commit_message>
<xml_diff>
--- a/variable names.xlsx
+++ b/variable names.xlsx
@@ -1,30 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kristen\Dropbox\Other\DBMI\BIST P8105\final project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryreyesnieva/Dropbox (Personal)/dbmi/coursework/Year 3/data_science/p8105_final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77223F35-43BE-1649-8363-ED0752F5CB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19035" windowHeight="6570"/>
+    <workbookView xWindow="8500" yWindow="460" windowWidth="29920" windowHeight="14860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="308">
   <si>
     <t>Variable Name</t>
   </si>
@@ -953,7 +962,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1300,23 +1309,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.53125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.19921875" customWidth="1"/>
+    <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1336,7 +1345,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1353,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1370,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1387,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1404,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1421,7 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1438,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1455,7 +1464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1472,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1489,7 +1498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1506,7 +1515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1523,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1540,7 +1549,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1557,7 +1566,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1591,7 +1600,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1608,7 +1617,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1625,7 +1634,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>58</v>
       </c>
@@ -1642,7 +1651,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
@@ -1659,7 +1668,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -1693,7 +1702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -1710,7 +1719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1727,7 +1736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -1744,7 +1753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -1761,7 +1770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -1778,7 +1787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -1795,7 +1804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -1812,7 +1821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>94</v>
       </c>
@@ -1829,7 +1838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>94</v>
       </c>
@@ -1846,7 +1855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -1863,7 +1872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>94</v>
       </c>
@@ -1880,7 +1889,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -1897,7 +1906,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -1917,7 +1926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -1934,7 +1943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -1951,7 +1960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -1968,7 +1977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -1985,7 +1994,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -2005,7 +2014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>94</v>
       </c>
@@ -2022,7 +2031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -2039,7 +2048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>94</v>
       </c>
@@ -2056,7 +2065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>94</v>
       </c>
@@ -2073,7 +2082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -2090,7 +2099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>94</v>
       </c>
@@ -2107,7 +2116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>94</v>
       </c>
@@ -2124,7 +2133,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -2141,7 +2150,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -2158,7 +2167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -2175,7 +2184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>143</v>
       </c>
@@ -2192,7 +2201,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>143</v>
       </c>
@@ -2206,7 +2215,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>143</v>
       </c>
@@ -2220,7 +2229,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>298</v>
       </c>
@@ -2237,7 +2246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>298</v>
       </c>
@@ -2254,7 +2263,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>298</v>
       </c>
@@ -2268,7 +2277,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>298</v>
       </c>
@@ -2285,7 +2294,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>298</v>
       </c>
@@ -2299,7 +2308,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>298</v>
       </c>
@@ -2316,7 +2325,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>298</v>
       </c>
@@ -2330,7 +2339,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>298</v>
       </c>
@@ -2347,7 +2356,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>298</v>
       </c>
@@ -2361,7 +2370,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>298</v>
       </c>
@@ -2375,7 +2384,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>298</v>
       </c>
@@ -2392,7 +2401,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>298</v>
       </c>
@@ -2409,7 +2418,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>158</v>
       </c>
@@ -2426,7 +2435,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>158</v>
       </c>
@@ -2440,7 +2449,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>158</v>
       </c>
@@ -2454,7 +2463,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>158</v>
       </c>
@@ -2468,7 +2477,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>158</v>
       </c>
@@ -2482,7 +2491,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>158</v>
       </c>
@@ -2496,7 +2505,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>158</v>
       </c>
@@ -2510,7 +2519,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>158</v>
       </c>
@@ -2524,7 +2533,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>158</v>
       </c>
@@ -2538,7 +2547,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>158</v>
       </c>
@@ -2552,7 +2561,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>158</v>
       </c>
@@ -2566,7 +2575,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>158</v>
       </c>
@@ -2580,7 +2589,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>158</v>
       </c>
@@ -2594,7 +2603,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>158</v>
       </c>
@@ -2608,7 +2617,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -2622,7 +2631,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>158</v>
       </c>
@@ -2636,7 +2645,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>158</v>
       </c>
@@ -2650,7 +2659,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>158</v>
       </c>
@@ -2664,7 +2673,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>158</v>
       </c>
@@ -2678,7 +2687,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>158</v>
       </c>
@@ -2692,7 +2701,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>158</v>
       </c>
@@ -2706,7 +2715,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>158</v>
       </c>
@@ -2720,7 +2729,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>158</v>
       </c>
@@ -2734,7 +2743,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>158</v>
       </c>
@@ -2748,7 +2757,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>158</v>
       </c>
@@ -2762,7 +2771,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>158</v>
       </c>
@@ -2776,7 +2785,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>158</v>
       </c>
@@ -2790,7 +2799,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>158</v>
       </c>
@@ -2804,7 +2813,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>158</v>
       </c>
@@ -2818,7 +2827,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>158</v>
       </c>
@@ -2832,7 +2841,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>158</v>
       </c>
@@ -2846,7 +2855,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>158</v>
       </c>
@@ -2860,7 +2869,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>158</v>
       </c>
@@ -2874,7 +2883,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>158</v>
       </c>
@@ -2888,7 +2897,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>158</v>
       </c>
@@ -2902,7 +2911,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>256</v>
       </c>
@@ -2916,7 +2925,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>256</v>
       </c>
@@ -2930,7 +2939,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>256</v>
       </c>
@@ -2944,7 +2953,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>256</v>
       </c>
@@ -2958,7 +2967,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>256</v>
       </c>
@@ -2972,7 +2981,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>256</v>
       </c>
@@ -2986,7 +2995,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>256</v>
       </c>
@@ -3000,7 +3009,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>256</v>
       </c>
@@ -3014,7 +3023,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>256</v>
       </c>
@@ -3028,7 +3037,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>256</v>
       </c>
@@ -3042,7 +3051,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>256</v>
       </c>
@@ -3056,7 +3065,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>256</v>
       </c>
@@ -3070,7 +3079,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>256</v>
       </c>
@@ -3084,7 +3093,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>256</v>
       </c>
@@ -3098,7 +3107,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>256</v>
       </c>
@@ -3112,7 +3121,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>256</v>
       </c>
@@ -3126,7 +3135,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>256</v>
       </c>
@@ -3140,7 +3149,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>256</v>
       </c>
@@ -3154,7 +3163,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>256</v>
       </c>
@@ -3168,7 +3177,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>256</v>
       </c>
@@ -3182,7 +3191,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>256</v>
       </c>
@@ -3196,7 +3205,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>256</v>
       </c>
@@ -3210,7 +3219,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>256</v>
       </c>
@@ -3224,7 +3233,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>256</v>
       </c>
@@ -3238,7 +3247,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>256</v>
       </c>
@@ -3252,7 +3261,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>256</v>
       </c>
@@ -3266,7 +3275,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>256</v>
       </c>
@@ -3280,7 +3289,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>256</v>
       </c>
@@ -3294,7 +3303,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>256</v>
       </c>
@@ -3308,7 +3317,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>256</v>
       </c>
@@ -3322,7 +3331,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>256</v>
       </c>
@@ -3336,7 +3345,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>256</v>
       </c>
@@ -3350,7 +3359,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>256</v>
       </c>
@@ -3364,7 +3373,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>256</v>
       </c>
@@ -3378,7 +3387,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>256</v>
       </c>
@@ -3396,4 +3405,1631 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC15705D-E7F5-854F-BD6F-3112B478C318}">
+  <dimension ref="A1:C134"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C134"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="str">
+        <f>CONCATENATE("`",B1,"` = ",LOWER(A1),",")</f>
+        <v>`Additions to the waiting list (annual count)` = wla_addcen_nc2,</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C65" si="0">CONCATENATE("`",B2,"` = ",LOWER(A2),",")</f>
+        <v>`Prevalent waitlist count (at beginning of year)` = wla_st_nc2,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>`Prevalent waitlist count (at end of year)` = wla_end_nc2,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>`Annual count of deceased donor transplants` = wla_remtxc_nc2,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>`Annual count of living donor transplants` = wla_remtxl_nc2,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>`Annual count of waitlist removals - deteriorated` = wla_remdet_nc2,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>`Annual count of waitlist removals - death` = wla_remdied_nc2,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of prevalent WL that received deceased donor transplant` = wla_remtxc_pcz,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of prevalent WL that received living donor transplant` = wla_remtxl_pcz,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of prevalent WL removed upon death` = wla_remdied_pcz,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of prevalent WL removed for deteriorating condition` = wla_remdet_pcz,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>`Offer Acceptance Ratio - Overall` = oa_overall_hr_mn_center,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>`Offer Acceptance Ratio - Low Risk Kidneys (KDRI &lt; 1.05)` = oa_lowrisk_hr_mn_center,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>`Offer Acceptance Ratio - Medium Risk Kidneys (1.05 &lt; KDRI &lt; 1.75)` = oa_mediumrisk_hr_mn_center,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>`Offer Acceptance Ratio - High Risk Kidneys (KDRI &gt; 1.75)` = oa_highrisk_hr_mn_center,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>`Offer Acceptance Ratio - Hard-to-Place Kidneys (&gt;100 offers)` = oa_hardtoplace100_hr_mn_center,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>`Offer Acceptance Ratio - Hard-to-Place Kidneys (&gt;100 offers)` = oa_hardtoplace_hr_mn_center,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>`Percent of deceased donor transplants from imported kidneys` = toc_shr_c,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>`Delayed Graft Function (dialysis in first week post-transplant)` = toc_wkdialy_c,</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Age &lt;2` = wlc_a2_allc2,</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Age 2-11` = wlc_a10_allc2,</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Age 12-17` = wlc_a17_allc2,</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Age 18-34` = wlc_a34_allc2,</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Age 35-49` = wlc_a49_allc2,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Age 50-64` = wlc_a64_allc2,</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Age 65+` = wlc_a65p_allc2,</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Age 65-69` = wlc_a69_allc2,</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Age 70+` = wlc_a70p_allc2,</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Male` = wlc_gm_allc2,</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Female` = wlc_gf_allc2,</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Asian Race` = wlc_ra_allc2,</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: African American Race` = wlc_rb_allc2,</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Hispanic/Latino Race` = wlc_rh_allc2,</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Other Race` = wlc_ro_allc2,</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Unknown Race` = wlc_ru_allc2,</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: White Race` = wlc_rw_allc2,</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: PRA &gt;= 80%` = wlc_pra80_allc2,</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: Previous Transplant = Yes` = wlc_ptxy_allc2,</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: ESKD cause = Diabetes` = wlc_kidia_allc2,</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: ESKD cause = glomerular disease` = wlc_kiglo_allc2,</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: ESKD cause = hypertensive nephrosclerosis` = wlc_kihyp_allc2,</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: ESKD cause = missing` = wlc_kimis_allc2,</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: ESKD cause = neoplasms` = wlc_kineo_allc2,</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: ESKD cause = other` = wlc_kioth_allc2,</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: ESKD cause = polycystic kidneys` = wlc_kipol_allc2,</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: ESKD cause = renovascular and vascular diseases` = wlc_kiren_allc2,</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: ESKD cause = retransplant/graft failure` = wlc_kirtr_allc2,</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: ESKD cause = tubular and interstitial diseases` = wlc_kitub_allc2,</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>`% of Prevalent WL: ESKD cause = congenital, familial, metabolic` = wlc_kicon_allc2,</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>`Median time to transplant` = ttt_50_c,</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>`25th percentile time to transplant` = ttt_25_c,</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>`75th percentile time to transplant` = ttt_75_c,</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>`Overall transplant rate (all candidates)` = tmr_txr_c2,</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B54" t="s">
+        <v>148</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>`Overall transplant rate (all candidates)` = tmr_txr_c,</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B55" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>`Overall transplant rate ratio (all candidates)` = tmr_txratio_c2,</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B56" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>`Overall transplant rate ratio (all candidates)` = tmr_txratio_c,</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B57" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>`Deceased donor transplant rate (all candidates)` = tmr_cadtxr_c2,</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B58" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>`Deceased donor transplant rate (all candidates)` = tmr_cadtx_r_c,</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B59" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>`Deceased donor transplant rate ratio (all candidates)` = tmr_cadtxratio_c2,</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B60" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>`Deceased donor transplant rate ratio (all candidates)` = tmr_cadtx_ratio_c,</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B61" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>`WL mortality rate (all candidates)` = tmr_dthr_c2,</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B62" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>`WL mortality rate ratio (all candidates)` = tmr_dthratio_c2,</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B63" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>`WL mortality rate (all candidates)` = tmr_dthr_c,</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B64" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>`WL mortality rate ratio (all candidates)` = tmr_dthratio_c,</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B65" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>`% DD TX recipients: Age &lt; 2` = rcc_a2_c,</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B66" t="s">
+        <v>176</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" ref="C66:C129" si="1">CONCATENATE("`",B66,"` = ",LOWER(A66),",")</f>
+        <v>`% DD TX recipients: Age 2-11` = rcc_a10_c,</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" t="s">
+        <v>175</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Age 12-17` = rcc_a17_c,</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B68" t="s">
+        <v>174</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Age 18-34` = rcc_a34_c,</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" t="s">
+        <v>173</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Age 35-49` = rcc_a49_c,</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" t="s">
+        <v>172</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Age 50-64` = rcc_a64_c,</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B71" t="s">
+        <v>171</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Age 65+` = rcc_a65p_c,</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B72" t="s">
+        <v>170</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Age 65-69` = rcc_a69_c,</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B73" t="s">
+        <v>169</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Age 70+` = rcc_a70p_c,</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B74" t="s">
+        <v>168</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Male` = rcc_gm_c,</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B75" t="s">
+        <v>167</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Female` = rcc_gf_c,</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B76" t="s">
+        <v>166</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Blood Type AB` = rcc_bab_c,</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B77" t="s">
+        <v>178</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Blood Type A` = rcc_ba_c,</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B78" t="s">
+        <v>179</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Blood Type B` = rcc_bb_c,</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B79" t="s">
+        <v>180</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: Blood Type O` = rcc_bo_c,</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B80" t="s">
+        <v>182</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: BMI 0-20` = rcc_bmi20_c,</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B81" t="s">
+        <v>183</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: BMI 21-25` = rcc_bmi25_c,</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B82" t="s">
+        <v>184</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: BMI 26-30` = rcc_bmi30_c,</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B83" t="s">
+        <v>219</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: BMI 31+` = rcc_bmi31p_c,</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B84" t="s">
+        <v>185</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: BMI 31-35` = rcc_bmi35_c,</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B85" t="s">
+        <v>186</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: BMI 36-40` = rcc_bmi40_c,</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B86" t="s">
+        <v>187</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>`% DD TX recipients: BMI 41+` = rcc_bmi41p_c,</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B87" t="s">
+        <v>203</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: ESKD cause = Diabetes` = rcc_dia_c,</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B88" t="s">
+        <v>204</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: glomerular disease` = rcc_glo_c,</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B89" t="s">
+        <v>205</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: hypertensive nephrosclerosis` = rcc_hyp_c,</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B90" t="s">
+        <v>206</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: missing` = rcc_mis_c,</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B91" t="s">
+        <v>207</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: neoplasms` = rcc_neo_c,</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="B92" t="s">
+        <v>208</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: other` = rcc_otk_c,</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B93" t="s">
+        <v>209</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: polycystic` = rcc_pol_c,</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B94" t="s">
+        <v>210</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: renovascular and vascular diseases` = rcc_vas_c,</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B95" t="s">
+        <v>211</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: retransplant/graft failure` = rcc_kiret_c,</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B96" t="s">
+        <v>212</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: tubular and interstitial diseases` = rcc_tub_c,</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B97" t="s">
+        <v>213</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: congenital, familial, metabolic` = rcc_con_c,</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B98" t="s">
+        <v>202</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: PRA &gt;= 80%` = rcc_pra80_c,</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B99" t="s">
+        <v>214</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of DD TX recipients: Previous TX = Yes` = rcc_ptxy_c,</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B100" t="s">
+        <v>221</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Age &lt; 2` = rcl_a2_c,</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B101" t="s">
+        <v>222</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Age 2-11` = rcl_a10_c,</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B102" t="s">
+        <v>223</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Age 12-17` = rcl_a17_c,</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B103" t="s">
+        <v>224</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Age 18-34` = rcl_a34_c,</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B104" t="s">
+        <v>225</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Age 35-49` = rcl_a49_c,</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B105" t="s">
+        <v>226</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Age 50-64` = rcl_a64_c,</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B106" t="s">
+        <v>227</v>
+      </c>
+      <c r="C106" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Age 65+` = rcl_a65p_c,</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B107" t="s">
+        <v>228</v>
+      </c>
+      <c r="C107" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Age 65-69` = rcl_a69_c,</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B108" t="s">
+        <v>229</v>
+      </c>
+      <c r="C108" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Age 70+` = rcl_a70p_c,</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B109" t="s">
+        <v>230</v>
+      </c>
+      <c r="C109" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Male` = rcl_gm_c,</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B110" t="s">
+        <v>231</v>
+      </c>
+      <c r="C110" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Female` = rcl_gf_c,</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="B111" t="s">
+        <v>232</v>
+      </c>
+      <c r="C111" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Blood Type AB` = rcl_bab_c,</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B112" t="s">
+        <v>233</v>
+      </c>
+      <c r="C112" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Blood Type A` = rcl_ba_c,</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B113" t="s">
+        <v>234</v>
+      </c>
+      <c r="C113" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Blood Type B` = rcl_bb_c,</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B114" t="s">
+        <v>235</v>
+      </c>
+      <c r="C114" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: Blood Type O` = rcl_bo_c,</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B115" t="s">
+        <v>236</v>
+      </c>
+      <c r="C115" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: BMI 0-20` = rcl_bmi20_c,</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B116" t="s">
+        <v>237</v>
+      </c>
+      <c r="C116" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: BMI 21-25` = rcl_bmi25_c,</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B117" t="s">
+        <v>238</v>
+      </c>
+      <c r="C117" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: BMI 26-30` = rcl_bmi30_c,</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B118" t="s">
+        <v>239</v>
+      </c>
+      <c r="C118" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: BMI 31+` = rcl_bmi31p_c,</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B119" t="s">
+        <v>240</v>
+      </c>
+      <c r="C119" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: BMI 31-35` = rcl_bmi35_c,</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B120" t="s">
+        <v>241</v>
+      </c>
+      <c r="C120" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: BMI 36-40` = rcl_bmi40_c,</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B121" t="s">
+        <v>242</v>
+      </c>
+      <c r="C121" t="str">
+        <f t="shared" si="1"/>
+        <v>`% LD TX recipients: BMI 41+` = rcl_bmi41p_c,</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="B122" t="s">
+        <v>243</v>
+      </c>
+      <c r="C122" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of LD TX recipients: ESKD cause = Diabetes` = rcl_dia_c,</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B123" t="s">
+        <v>244</v>
+      </c>
+      <c r="C123" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of LD TX recipients: glomerular disease` = rcl_glo_c,</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="B124" t="s">
+        <v>255</v>
+      </c>
+      <c r="C124" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of LD TX recipients: hypertensive nephrosclerosis` = rcl_hyp_c,</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B125" t="s">
+        <v>254</v>
+      </c>
+      <c r="C125" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of LD TX recipients: missing` = rcl_mis_c,</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="B126" t="s">
+        <v>253</v>
+      </c>
+      <c r="C126" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of LD TX recipients: neoplasms` = rcl_neo_c,</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B127" t="s">
+        <v>252</v>
+      </c>
+      <c r="C127" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of LD TX recipients: other` = rcl_otk_c,</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B128" t="s">
+        <v>251</v>
+      </c>
+      <c r="C128" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of LD TX recipients: polycystic` = rcl_pol_c,</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B129" t="s">
+        <v>250</v>
+      </c>
+      <c r="C129" t="str">
+        <f t="shared" si="1"/>
+        <v>`% of LD TX recipients: renovascular and vascular diseases` = rcl_vas_c,</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B130" t="s">
+        <v>249</v>
+      </c>
+      <c r="C130" t="str">
+        <f t="shared" ref="C130:C134" si="2">CONCATENATE("`",B130,"` = ",LOWER(A130),",")</f>
+        <v>`% of LD TX recipients: retransplant/graft failure` = rcl_ret_c,</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B131" t="s">
+        <v>248</v>
+      </c>
+      <c r="C131" t="str">
+        <f t="shared" si="2"/>
+        <v>`% of LD TX recipients: tubular and interstitial diseases` = rcl_tub_c,</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B132" t="s">
+        <v>247</v>
+      </c>
+      <c r="C132" t="str">
+        <f t="shared" si="2"/>
+        <v>`% of LD TX recipients: congenital, familial, metabolic` = rcl_con_c,</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B133" t="s">
+        <v>246</v>
+      </c>
+      <c r="C133" t="str">
+        <f t="shared" si="2"/>
+        <v>`% of LD TX recipients: PRA &gt;= 80%` = rcl_pra80_c,</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B134" t="s">
+        <v>245</v>
+      </c>
+      <c r="C134" t="str">
+        <f t="shared" si="2"/>
+        <v>`% of LD TX recipients: Previous TX = Yes` = rcl_ptxy_c,</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>